<commit_message>
add mean and regression line
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD880352-6AD5-7C4D-957D-48E45BE353A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C3759E-8F49-8D4A-8424-A660F97CD16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,9 +421,6 @@
     <t>16-jarige scholieren</t>
   </si>
   <si>
-    <t>basisschoolleerlingen van groep 8</t>
-  </si>
-  <si>
     <t>21-jarige studenten</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>1982 en 1987</t>
+  </si>
+  <si>
+    <t>leerlingen van groep 8</t>
   </si>
 </sst>
 </file>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B15CAE-7079-3347-9EA7-135DB64C084D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -893,13 +893,13 @@
         <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -916,10 +916,10 @@
         <v>78</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -936,10 +936,10 @@
         <v>78</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -956,10 +956,10 @@
         <v>78</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -973,13 +973,13 @@
         <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -993,13 +993,13 @@
         <v>85</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1013,13 +1013,13 @@
         <v>86</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1033,13 +1033,13 @@
         <v>87</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1053,13 +1053,13 @@
         <v>88</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1073,13 +1073,13 @@
         <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1093,13 +1093,13 @@
         <v>90</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1113,13 +1113,13 @@
         <v>91</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1133,13 +1133,13 @@
         <v>92</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1153,13 +1153,13 @@
         <v>93</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1173,13 +1173,13 @@
         <v>94</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1193,13 +1193,13 @@
         <v>111</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1213,13 +1213,13 @@
         <v>112</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,13 +1233,13 @@
         <v>113</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1256,10 +1256,10 @@
         <v>127</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1276,10 +1276,10 @@
         <v>127</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1296,10 +1296,10 @@
         <v>127</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1316,10 +1316,10 @@
         <v>127</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1336,10 +1336,10 @@
         <v>127</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1356,10 +1356,10 @@
         <v>127</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1373,13 +1373,13 @@
         <v>115</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1393,13 +1393,13 @@
         <v>114</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1413,13 +1413,13 @@
         <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1436,10 +1436,10 @@
         <v>79</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1456,10 +1456,10 @@
         <v>79</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1476,10 +1476,10 @@
         <v>79</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1496,10 +1496,10 @@
         <v>79</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1516,10 +1516,10 @@
         <v>79</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1536,10 +1536,10 @@
         <v>79</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1556,10 +1556,10 @@
         <v>79</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1576,10 +1576,10 @@
         <v>79</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1596,10 +1596,10 @@
         <v>79</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1610,16 +1610,16 @@
         <v>63</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1630,16 +1630,16 @@
         <v>65</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1650,16 +1650,16 @@
         <v>67</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1670,16 +1670,16 @@
         <v>69</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1696,10 +1696,10 @@
         <v>79</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1716,10 +1716,10 @@
         <v>79</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1736,10 +1736,10 @@
         <v>79</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1756,10 +1756,10 @@
         <v>79</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add switch button for showing one or two groups
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C172B912-E692-FA45-BA84-9B66EFEE8E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29646A0-3E93-7947-A3BF-44915F1E2DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="-31920" yWindow="-1940" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -338,9 +338,6 @@
     <t>Een hoogst behaalde onderwijsniveau van tenminste WO-Bachelor.</t>
   </si>
   <si>
-    <t>Het gemiddelde bruto inkomen tussen 2017 en 2018 gemeten in 2018 euros.</t>
-  </si>
-  <si>
     <t>Het gemiddelde uurloon in 2018 euros. Uurloon wordt berekend door het basisloon over 2017-2018 te delen door de som van het aantal basisuren.</t>
   </si>
   <si>
@@ -687,6 +684,9 @@
   </si>
   <si>
     <t>Wijk</t>
+  </si>
+  <si>
+    <t>het gemiddelde bruto jaarinkomen 2017 en 2018 (prijspeil van 2018)</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B15CAE-7079-3347-9EA7-135DB64C084D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1116,19 +1116,19 @@
         <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>82</v>
@@ -1148,10 +1148,10 @@
         <v>78</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>83</v>
@@ -1171,10 +1171,10 @@
         <v>78</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1182,22 +1182,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1208,19 +1208,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1231,19 +1231,19 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>85</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1254,19 +1254,19 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>86</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1277,19 +1277,19 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1300,19 +1300,19 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>88</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1323,19 +1323,19 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>89</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1346,19 +1346,19 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1369,19 +1369,19 @@
         <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1392,19 +1392,19 @@
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>92</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1415,19 +1415,19 @@
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1438,19 +1438,19 @@
         <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>94</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1458,22 +1458,22 @@
         <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1481,22 +1481,22 @@
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1504,22 +1504,22 @@
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1530,19 +1530,19 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>95</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1553,19 +1553,19 @@
         <v>33</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1576,19 +1576,19 @@
         <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>97</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1596,22 +1596,22 @@
         <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1619,22 +1619,22 @@
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1642,22 +1642,22 @@
         <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1668,19 +1668,19 @@
         <v>40</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1691,19 +1691,19 @@
         <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1714,19 +1714,19 @@
         <v>44</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1734,22 +1734,22 @@
         <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1760,7 +1760,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>98</v>
@@ -1769,10 +1769,10 @@
         <v>79</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1783,7 +1783,7 @@
         <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>99</v>
@@ -1792,10 +1792,10 @@
         <v>79</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1806,19 +1806,19 @@
         <v>51</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -1829,19 +1829,19 @@
         <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1852,19 +1852,19 @@
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1875,19 +1875,19 @@
         <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1898,19 +1898,19 @@
         <v>59</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1921,19 +1921,19 @@
         <v>61</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1944,19 +1944,19 @@
         <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1967,19 +1967,19 @@
         <v>65</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1990,19 +1990,19 @@
         <v>67</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -2013,19 +2013,19 @@
         <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -2036,19 +2036,19 @@
         <v>71</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2059,19 +2059,19 @@
         <v>73</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2079,22 +2079,22 @@
         <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2105,19 +2105,19 @@
         <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2133,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8C81BE-EE76-9E4A-98BE-73EF8C350CA9}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="166" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2145,514 +2145,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B62" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change circles to squares
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989B31AF-DE28-4C4A-BC57-3507A6B4A6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD6E539-D419-6044-AEDB-3187F811A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1900" windowWidth="38400" windowHeight="21100" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>c21_high_school_attained</t>
   </si>
   <si>
-    <t>Startkwalificatie</t>
-  </si>
-  <si>
     <t>21-jarige studenten</t>
   </si>
   <si>
@@ -334,18 +331,12 @@
     <t>c21_hbo_followed</t>
   </si>
   <si>
-    <t>Volgt hbo of hoger</t>
-  </si>
-  <si>
     <t>het percentage 21-jarigen dat hbo en/of wo heeft gevolgd.</t>
   </si>
   <si>
     <t>C21_uni_followed</t>
   </si>
   <si>
-    <t>Volgt universiteit</t>
-  </si>
-  <si>
     <t>het percentage 21-jarigen dat wo heeft gevolgd.</t>
   </si>
   <si>
@@ -689,6 +680,15 @@
   </si>
   <si>
     <t>Wonen</t>
+  </si>
+  <si>
+    <t>Startkwalificatie behaald</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd hbo of hoger</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd universiteit</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B15CAE-7079-3347-9EA7-135DB64C084D}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1159,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -1182,7 +1182,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
@@ -1205,7 +1205,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
@@ -1229,7 +1229,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>23</v>
@@ -1252,7 +1252,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -1275,7 +1275,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>32</v>
@@ -1298,7 +1298,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>35</v>
@@ -1321,7 +1321,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>40</v>
@@ -1344,7 +1344,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>43</v>
@@ -1367,7 +1367,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>46</v>
@@ -1390,7 +1390,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>49</v>
@@ -1413,7 +1413,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>52</v>
@@ -1436,7 +1436,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>55</v>
@@ -1459,7 +1459,7 @@
         <v>57</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>58</v>
@@ -1482,7 +1482,7 @@
         <v>60</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>61</v>
@@ -1505,7 +1505,7 @@
         <v>63</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>64</v>
@@ -1528,7 +1528,7 @@
         <v>66</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>67</v>
@@ -1551,7 +1551,7 @@
         <v>69</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>67</v>
@@ -1574,7 +1574,7 @@
         <v>71</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>72</v>
@@ -1597,7 +1597,7 @@
         <v>74</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>75</v>
@@ -1620,7 +1620,7 @@
         <v>77</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>78</v>
@@ -1643,7 +1643,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>81</v>
@@ -1666,7 +1666,7 @@
         <v>83</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>84</v>
@@ -1689,7 +1689,7 @@
         <v>86</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>87</v>
@@ -1712,7 +1712,7 @@
         <v>89</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>90</v>
@@ -1735,7 +1735,7 @@
         <v>92</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>93</v>
@@ -1755,16 +1755,16 @@
         <v>94</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>30</v>
@@ -1775,19 +1775,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>30</v>
@@ -1798,19 +1798,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>217</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>30</v>
@@ -1821,16 +1821,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>38</v>
@@ -1844,16 +1844,16 @@
     </row>
     <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>38</v>
@@ -1867,16 +1867,16 @@
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>38</v>
@@ -1890,16 +1890,16 @@
     </row>
     <row r="34" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>38</v>
@@ -1913,16 +1913,16 @@
     </row>
     <row r="35" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>38</v>
@@ -1936,16 +1936,16 @@
     </row>
     <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>38</v>
@@ -1959,16 +1959,16 @@
     </row>
     <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>38</v>
@@ -1982,16 +1982,16 @@
     </row>
     <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>38</v>
@@ -2005,16 +2005,16 @@
     </row>
     <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>38</v>
@@ -2028,16 +2028,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>38</v>
@@ -2051,16 +2051,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>38</v>
@@ -2074,16 +2074,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>20</v>
@@ -2097,16 +2097,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>29</v>
@@ -2120,16 +2120,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>38</v>
@@ -2163,514 +2163,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tooltip to opleiding ouders although it doesnt work
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD6E539-D419-6044-AEDB-3187F811A000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800E0E58-4E53-3D47-8337-FC8E4E4A3E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
-    <sheet name="outcome" sheetId="1" r:id="rId1"/>
+    <sheet name="outcome" sheetId="3" r:id="rId1"/>
     <sheet name="area" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -695,7 +695,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -714,12 +714,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -777,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -787,14 +781,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,27 +1103,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B15CAE-7079-3347-9EA7-135DB64C084D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D204B-9EFA-3D41-9D75-AECB47552519}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" style="2" customWidth="1"/>
-    <col min="4" max="4" width="60" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="112.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="3"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1151,137 +1146,136 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>213</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>213</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>29</v>
+        <v>213</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>30</v>
@@ -1290,21 +1284,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>213</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>30</v>
@@ -1313,18 +1307,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>40</v>
+        <v>213</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>38</v>
@@ -1333,21 +1327,21 @@
         <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>43</v>
+        <v>213</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>38</v>
@@ -1356,21 +1350,21 @@
         <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>46</v>
+      <c r="D11" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>38</v>
@@ -1382,7 +1376,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1405,18 +1399,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>211</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>38</v>
@@ -1428,41 +1422,41 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>58</v>
+        <v>211</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>20</v>
@@ -1474,41 +1468,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>20</v>
+        <v>211</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>211</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>20</v>
@@ -1520,435 +1514,436 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>20</v>
+        <v>211</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>86</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>29</v>
+        <v>67</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>29</v>
+        <v>67</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>94</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>96</v>
+      <c r="D28" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>97</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>216</v>
+        <v>54</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>99</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>217</v>
+        <v>60</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>104</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>212</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>109</v>
+        <v>212</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>110</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>113</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>116</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>118</v>
+        <v>212</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>30</v>
@@ -1957,21 +1952,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>119</v>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>30</v>
@@ -1980,21 +1975,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>122</v>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>30</v>
@@ -2003,21 +1998,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>126</v>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>38</v>
+        <v>87</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>30</v>
@@ -2027,20 +2022,20 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>137</v>
+      <c r="A40" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>38</v>
+        <v>212</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>30</v>
@@ -2050,20 +2045,20 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>128</v>
+      <c r="A41" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>38</v>
+        <v>212</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>30</v>
@@ -2073,66 +2068,66 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>131</v>
+      <c r="A42" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>214</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>134</v>
+      <c r="A43" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>214</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>29</v>
+        <v>133</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>214</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>38</v>
+        <v>136</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>30</v>
@@ -2142,7 +2137,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add highlighted points and fix some errors on the server
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800E0E58-4E53-3D47-8337-FC8E4E4A3E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877A8660-DF58-C54D-AE06-77755379E7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -94,601 +94,601 @@
     <t>c11_youth_health_costs</t>
   </si>
   <si>
+    <t>leerlingen van groep 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700 duizend </t>
+  </si>
+  <si>
+    <t>2003-2006</t>
+  </si>
+  <si>
+    <t>gemiddelde totale zorgkosten, vergoed vanuit de Zorgverzekeringswet, van leerlingen in groep 8 in het kalenderjaar waarin zij de eindtoets deden.</t>
+  </si>
+  <si>
+    <t>c11_youth_protection</t>
+  </si>
+  <si>
+    <t>het percentage leerlingen in groep 8 met een jeugdbeschermingsmaatregel in het kalenderjaar van de eindtoets in groep 8.</t>
+  </si>
+  <si>
+    <t>c16_youth_health_costs</t>
+  </si>
+  <si>
+    <t>16-jarige scholieren</t>
+  </si>
+  <si>
+    <t>1 miljoen</t>
+  </si>
+  <si>
+    <t>1998-2002</t>
+  </si>
+  <si>
+    <t>gemiddelde totale zorgkosten, vergoed vanuit de Zorgverzekeringswet, van 16-jarigen in het jaar dat zij 16 werden.</t>
+  </si>
+  <si>
+    <t>c16_youth_protection</t>
+  </si>
+  <si>
+    <t>het percentage 16-jarigen met een jeugdbeschermingsmaatregel in het jaar dat ze 16 werden.</t>
+  </si>
+  <si>
+    <t>c30_total_health_costs</t>
+  </si>
+  <si>
+    <t>Zorgkosten</t>
+  </si>
+  <si>
+    <t>dertigers</t>
+  </si>
+  <si>
+    <t>1982-1987</t>
+  </si>
+  <si>
+    <t>gemiddelde totale zorgkosten in 2018.</t>
+  </si>
+  <si>
+    <t>c30_basic_mhc</t>
+  </si>
+  <si>
+    <t>Geestelijke gezondheidszorg (basis)</t>
+  </si>
+  <si>
+    <t>het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (basis), vergoed vanuit de Zorgverzekeringswet.</t>
+  </si>
+  <si>
+    <t>c30_specialist_mhc</t>
+  </si>
+  <si>
+    <t>Geestelijke gezondheidszorg (specialistisch)</t>
+  </si>
+  <si>
+    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (specialistisch), vergoed vanuit de Zorgverzekeringswet.</t>
+  </si>
+  <si>
+    <t>c30_hospital</t>
+  </si>
+  <si>
+    <t>Gebruikt ziekenhuiszorg</t>
+  </si>
+  <si>
+    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van ziekenhuiszorg, vergoed vanuit de Zorgverzekeringswet.</t>
+  </si>
+  <si>
+    <t>c30_pharma</t>
+  </si>
+  <si>
+    <t>Gebruikt medicijnen</t>
+  </si>
+  <si>
+    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van medicijnen, vergoed vanuit de Zorgverzekeringswet.</t>
+  </si>
+  <si>
+    <t>c11_vmbo_gl_test</t>
+  </si>
+  <si>
+    <t>Eindtoetsadvies vmbo-GL en hoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van tenminste vmbo gemengde leerweg. </t>
+  </si>
+  <si>
+    <t>c11_havo_test</t>
+  </si>
+  <si>
+    <t>Eindtoetsadvies havo en hoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van tenminste havo. </t>
+  </si>
+  <si>
+    <t>c11_vwo_test</t>
+  </si>
+  <si>
+    <t>Eindtoetsadvies vwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van vwo. </t>
+  </si>
+  <si>
+    <t>c11_math</t>
+  </si>
+  <si>
+    <t>Eindtoets rekenen streefniveau</t>
+  </si>
+  <si>
+    <t>het percentage leerlingen in groep 8 met een rekenscore van tenminste het streefniveau (1S of 2F) op de eindtoets.</t>
+  </si>
+  <si>
+    <t>c11_reading</t>
+  </si>
+  <si>
+    <t>Eindtoets lezen streefniveau</t>
+  </si>
+  <si>
+    <t>het percentage  leerlingen in groep 8 met een taalvaardigheidscore van tenminste het streefniveau (2F) op de eindtoets.</t>
+  </si>
+  <si>
+    <t>c11_language</t>
+  </si>
+  <si>
+    <t>Eindtoets taalverzorging streefniveau</t>
+  </si>
+  <si>
+    <t>c11_vmbo_gl_final</t>
+  </si>
+  <si>
+    <t>Schooladvies vmbo-GL en hoger</t>
+  </si>
+  <si>
+    <t>het percentage leerlingen in groep 8 met een schooladvies van tenminste vmbo gemengde leerweg.</t>
+  </si>
+  <si>
+    <t>c11_havo_final</t>
+  </si>
+  <si>
+    <t>Schooladvies havo en hoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies van tenminste havo. </t>
+  </si>
+  <si>
+    <t>c11_vwo_final</t>
+  </si>
+  <si>
+    <t>Schooladvies vwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage kinderen met een schooladvies van vwo. </t>
+  </si>
+  <si>
+    <t>c11_over_advice</t>
+  </si>
+  <si>
+    <t>Schooladvies hoger dan eindtoetsadvies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies dat tenminste één niveau hoger is dan het eindtoetsadvies. </t>
+  </si>
+  <si>
+    <t>c11_under_advice</t>
+  </si>
+  <si>
+    <t>Schooladvies lager dan eindtoetsadvies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies dat tenminste één niveau lager is dan het eindtoetsadvies. </t>
+  </si>
+  <si>
+    <t>c16_vmbo_gl</t>
+  </si>
+  <si>
+    <t>Volgt vmbo-GL of hoger</t>
+  </si>
+  <si>
+    <t>het percentage 16-jarigen dat tenminste vmbo gemengde leerweg of hoger heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>c16_havo</t>
+  </si>
+  <si>
+    <t>Volgt havo of hoger</t>
+  </si>
+  <si>
+    <t>het percentage 16-jarigen dat tenminste havo heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>c16_vwo</t>
+  </si>
+  <si>
+    <t>Volgt vwo</t>
+  </si>
+  <si>
+    <t>het percentage 16-jarigen dat vwo heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>c21_high_school_attained</t>
+  </si>
+  <si>
+    <t>21-jarige studenten</t>
+  </si>
+  <si>
+    <t>het percentage 21-jarigen dat een startkwalificatie heeft behaald (havo, vwo, of mbo niveau 2 of hoger).</t>
+  </si>
+  <si>
+    <t>c21_hbo_followed</t>
+  </si>
+  <si>
+    <t>het percentage 21-jarigen dat hbo en/of wo heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>C21_uni_followed</t>
+  </si>
+  <si>
+    <t>het percentage 21-jarigen dat wo heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>c30_hbo_attained</t>
+  </si>
+  <si>
+    <t>Diploma hbo of hoger</t>
+  </si>
+  <si>
+    <t>het percentage dertigers dat tenminste een hbo-diploma heeft behaald.</t>
+  </si>
+  <si>
+    <t>c30_wo_attained</t>
+  </si>
+  <si>
+    <t>Diploma universiteit</t>
+  </si>
+  <si>
+    <t>het percentage 21-jarigen dat tenminste een wo bachelordiploma heeft behaald.</t>
+  </si>
+  <si>
+    <t>c30_income</t>
+  </si>
+  <si>
+    <t>Persoonlijk inkomen</t>
+  </si>
+  <si>
+    <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
+  </si>
+  <si>
+    <t>c30_hourly_wage</t>
+  </si>
+  <si>
+    <t>Uurloon</t>
+  </si>
+  <si>
+    <t>het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017-2018 te delen door het aantal gewerkte basisuren.</t>
+  </si>
+  <si>
+    <t>c30_hrs_work_pw</t>
+  </si>
+  <si>
+    <t>Uren werk per week</t>
+  </si>
+  <si>
+    <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst, berekend door het aantal gewerkte basisuren in 2017 en 2018 te delen door 104.</t>
+  </si>
+  <si>
+    <t>c30_flex_contract</t>
+  </si>
+  <si>
+    <t>Flexibel arbeidscontract</t>
+  </si>
+  <si>
+    <t>het percentage dertigers in loondienst dat geen contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
+  </si>
+  <si>
+    <t>c30_employed</t>
+  </si>
+  <si>
+    <t>Werkend</t>
+  </si>
+  <si>
+    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
+  </si>
+  <si>
+    <t>c30_social_assistance</t>
+  </si>
+  <si>
+    <t>Bijstand</t>
+  </si>
+  <si>
+    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
+  </si>
+  <si>
+    <t>c30_disability</t>
+  </si>
+  <si>
+    <t>Uitkering arbeidsongeschiktheid/ziekte</t>
+  </si>
+  <si>
+    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
+  </si>
+  <si>
+    <t>c30_debt</t>
+  </si>
+  <si>
+    <t>Schulden</t>
+  </si>
+  <si>
+    <t>het percentage dertigers met een negatief vermogen.</t>
+  </si>
+  <si>
+    <t>c11_living_space_pp</t>
+  </si>
+  <si>
+    <t>het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8</t>
+  </si>
+  <si>
+    <t>c16_living_space_pp</t>
+  </si>
+  <si>
+    <t>het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
+  </si>
+  <si>
+    <t>c30_wealth</t>
+  </si>
+  <si>
+    <t>Vermogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertiger behoren in 2018. </t>
+  </si>
+  <si>
+    <t>c30_home_owner</t>
+  </si>
+  <si>
+    <t>Huiseigenaar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het percentage dertigers met een koophuis in is eigenaar van een huis. </t>
+  </si>
+  <si>
+    <t>geografie</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Nederland</t>
+  </si>
+  <si>
+    <t>Metropool Amsterdam</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Gemeente</t>
+  </si>
+  <si>
+    <t>Almere</t>
+  </si>
+  <si>
+    <t>Amstelveen</t>
+  </si>
+  <si>
+    <t>Beverwijk</t>
+  </si>
+  <si>
+    <t>Gooise Meren</t>
+  </si>
+  <si>
+    <t>Haarlem</t>
+  </si>
+  <si>
+    <t>Haarlemmermeer</t>
+  </si>
+  <si>
+    <t>Lelystad</t>
+  </si>
+  <si>
+    <t>Purmerend</t>
+  </si>
+  <si>
+    <t>Velsen</t>
+  </si>
+  <si>
+    <t>Zaanstad</t>
+  </si>
+  <si>
+    <t>Edam-Volendam</t>
+  </si>
+  <si>
+    <t>Aalsmeer</t>
+  </si>
+  <si>
+    <t>Heemskerk</t>
+  </si>
+  <si>
+    <t>Hilversum</t>
+  </si>
+  <si>
+    <t>Huizen</t>
+  </si>
+  <si>
+    <t>Uithoorn</t>
+  </si>
+  <si>
+    <t>Bloemendaal</t>
+  </si>
+  <si>
+    <t>Heemstede</t>
+  </si>
+  <si>
+    <t>Wijdemeren</t>
+  </si>
+  <si>
+    <t>Wormerland</t>
+  </si>
+  <si>
+    <t>Diemen</t>
+  </si>
+  <si>
+    <t>Waterland</t>
+  </si>
+  <si>
+    <t>Weesp</t>
+  </si>
+  <si>
+    <t>Zuidoost</t>
+  </si>
+  <si>
+    <t>Stadsdeel</t>
+  </si>
+  <si>
+    <t>Noord</t>
+  </si>
+  <si>
+    <t>Oost</t>
+  </si>
+  <si>
+    <t>Nieuw-West</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Centrum</t>
+  </si>
+  <si>
+    <t>Zuid</t>
+  </si>
+  <si>
+    <t>Gaasperdam, Driemond</t>
+  </si>
+  <si>
+    <t>Wijk</t>
+  </si>
+  <si>
+    <t>Noord-Oost</t>
+  </si>
+  <si>
+    <t>Bijlmer-Centrum, Amstel III</t>
+  </si>
+  <si>
+    <t>Indische Buurt, Oostelijk Havengebied</t>
+  </si>
+  <si>
+    <t>De Pijp, Rivierenbuurt</t>
+  </si>
+  <si>
+    <t>De Aker, Sloten, Nieuw-Sloten</t>
+  </si>
+  <si>
+    <t>Geuzenveld, Slotermeer, Sloterdijken</t>
+  </si>
+  <si>
+    <t>Osdorp</t>
+  </si>
+  <si>
+    <t>Bijlmer-Oost</t>
+  </si>
+  <si>
+    <t>Oud-Oost</t>
+  </si>
+  <si>
+    <t>Slotervaart</t>
+  </si>
+  <si>
+    <t>Noord-West</t>
+  </si>
+  <si>
+    <t>Bos en Lommer</t>
+  </si>
+  <si>
+    <t>IJburg, Zeeburgereiland</t>
+  </si>
+  <si>
+    <t>Oud West, De Baarsjes</t>
+  </si>
+  <si>
+    <t>Oud-Zuid</t>
+  </si>
+  <si>
+    <t>Oud-Noord</t>
+  </si>
+  <si>
+    <t>Westerpark</t>
+  </si>
+  <si>
+    <t>Centrum-Oost</t>
+  </si>
+  <si>
+    <t>Watergraafsmeer</t>
+  </si>
+  <si>
+    <t>Uitgeest</t>
+  </si>
+  <si>
+    <t>Zandvoort</t>
+  </si>
+  <si>
+    <t>Ouder-Amstel</t>
+  </si>
+  <si>
+    <t>Beemster</t>
+  </si>
+  <si>
+    <t>Landsmeer</t>
+  </si>
+  <si>
+    <t>Oostzaan</t>
+  </si>
+  <si>
+    <t>Blaricum</t>
+  </si>
+  <si>
+    <t>Laren</t>
+  </si>
+  <si>
+    <t>Centrum-West</t>
+  </si>
+  <si>
+    <t>Buitenveldert, Zuidas</t>
+  </si>
+  <si>
+    <t>Gezondheid en Welzijn</t>
+  </si>
+  <si>
+    <t>Onderwijs</t>
+  </si>
+  <si>
+    <t>Geld</t>
+  </si>
+  <si>
+    <t>Wonen</t>
+  </si>
+  <si>
+    <t>Startkwalificatie behaald</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd hbo of hoger</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd universiteit</t>
+  </si>
+  <si>
+    <t>Woonoppervlak per lid van kinderen</t>
+  </si>
+  <si>
+    <t>Woonoppervlak per lid van tieners</t>
+  </si>
+  <si>
     <t>Jeugd zorgkosten van kinderen</t>
   </si>
   <si>
-    <t>leerlingen van groep 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">700 duizend </t>
-  </si>
-  <si>
-    <t>2003-2006</t>
-  </si>
-  <si>
-    <t>gemiddelde totale zorgkosten, vergoed vanuit de Zorgverzekeringswet, van leerlingen in groep 8 in het kalenderjaar waarin zij de eindtoets deden.</t>
-  </si>
-  <si>
-    <t>c11_youth_protection</t>
+    <t>Jeugd zorgkosten van tieners</t>
   </si>
   <si>
     <t>Jeugdbescherming van kinderen</t>
   </si>
   <si>
-    <t>het percentage leerlingen in groep 8 met een jeugdbeschermingsmaatregel in het kalenderjaar van de eindtoets in groep 8.</t>
-  </si>
-  <si>
-    <t>c16_youth_health_costs</t>
-  </si>
-  <si>
-    <t>Jeugd zorgkosten van tieners</t>
-  </si>
-  <si>
-    <t>16-jarige scholieren</t>
-  </si>
-  <si>
-    <t>1 miljoen</t>
-  </si>
-  <si>
-    <t>1998-2002</t>
-  </si>
-  <si>
-    <t>gemiddelde totale zorgkosten, vergoed vanuit de Zorgverzekeringswet, van 16-jarigen in het jaar dat zij 16 werden.</t>
-  </si>
-  <si>
-    <t>c16_youth_protection</t>
-  </si>
-  <si>
     <t>Jeugdbescherming van tieners</t>
-  </si>
-  <si>
-    <t>het percentage 16-jarigen met een jeugdbeschermingsmaatregel in het jaar dat ze 16 werden.</t>
-  </si>
-  <si>
-    <t>c30_total_health_costs</t>
-  </si>
-  <si>
-    <t>Zorgkosten</t>
-  </si>
-  <si>
-    <t>dertigers</t>
-  </si>
-  <si>
-    <t>1982-1987</t>
-  </si>
-  <si>
-    <t>gemiddelde totale zorgkosten in 2018.</t>
-  </si>
-  <si>
-    <t>c30_basic_mhc</t>
-  </si>
-  <si>
-    <t>Geestelijke gezondheidszorg (basis)</t>
-  </si>
-  <si>
-    <t>het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (basis), vergoed vanuit de Zorgverzekeringswet.</t>
-  </si>
-  <si>
-    <t>c30_specialist_mhc</t>
-  </si>
-  <si>
-    <t>Geestelijke gezondheidszorg (specialistisch)</t>
-  </si>
-  <si>
-    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (specialistisch), vergoed vanuit de Zorgverzekeringswet.</t>
-  </si>
-  <si>
-    <t>c30_hospital</t>
-  </si>
-  <si>
-    <t>Gebruikt ziekenhuiszorg</t>
-  </si>
-  <si>
-    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van ziekenhuiszorg, vergoed vanuit de Zorgverzekeringswet.</t>
-  </si>
-  <si>
-    <t>c30_pharma</t>
-  </si>
-  <si>
-    <t>Gebruikt medicijnen</t>
-  </si>
-  <si>
-    <t>Het percentage van dertigers dat in 2018 gebruikt maakte van medicijnen, vergoed vanuit de Zorgverzekeringswet.</t>
-  </si>
-  <si>
-    <t>c11_vmbo_gl_test</t>
-  </si>
-  <si>
-    <t>Eindtoetsadvies vmbo-GL en hoger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van tenminste vmbo gemengde leerweg. </t>
-  </si>
-  <si>
-    <t>c11_havo_test</t>
-  </si>
-  <si>
-    <t>Eindtoetsadvies havo en hoger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van tenminste havo. </t>
-  </si>
-  <si>
-    <t>c11_vwo_test</t>
-  </si>
-  <si>
-    <t>Eindtoetsadvies vwo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een eindtoetsadvies van vwo. </t>
-  </si>
-  <si>
-    <t>c11_math</t>
-  </si>
-  <si>
-    <t>Eindtoets rekenen streefniveau</t>
-  </si>
-  <si>
-    <t>het percentage leerlingen in groep 8 met een rekenscore van tenminste het streefniveau (1S of 2F) op de eindtoets.</t>
-  </si>
-  <si>
-    <t>c11_reading</t>
-  </si>
-  <si>
-    <t>Eindtoets lezen streefniveau</t>
-  </si>
-  <si>
-    <t>het percentage  leerlingen in groep 8 met een taalvaardigheidscore van tenminste het streefniveau (2F) op de eindtoets.</t>
-  </si>
-  <si>
-    <t>c11_language</t>
-  </si>
-  <si>
-    <t>Eindtoets taalverzorging streefniveau</t>
-  </si>
-  <si>
-    <t>c11_vmbo_gl_final</t>
-  </si>
-  <si>
-    <t>Schooladvies vmbo-GL en hoger</t>
-  </si>
-  <si>
-    <t>het percentage leerlingen in groep 8 met een schooladvies van tenminste vmbo gemengde leerweg.</t>
-  </si>
-  <si>
-    <t>c11_havo_final</t>
-  </si>
-  <si>
-    <t>Schooladvies havo en hoger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies van tenminste havo. </t>
-  </si>
-  <si>
-    <t>c11_vwo_final</t>
-  </si>
-  <si>
-    <t>Schooladvies vwo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage kinderen met een schooladvies van vwo. </t>
-  </si>
-  <si>
-    <t>c11_over_advice</t>
-  </si>
-  <si>
-    <t>Schooladvies hoger dan eindtoetsadvies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies dat tenminste één niveau hoger is dan het eindtoetsadvies. </t>
-  </si>
-  <si>
-    <t>c11_under_advice</t>
-  </si>
-  <si>
-    <t>Schooladvies lager dan eindtoetsadvies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het percentage leerlingen in groep 8 met een schooladvies dat tenminste één niveau lager is dan het eindtoetsadvies. </t>
-  </si>
-  <si>
-    <t>c16_vmbo_gl</t>
-  </si>
-  <si>
-    <t>Volgt vmbo-GL of hoger</t>
-  </si>
-  <si>
-    <t>het percentage 16-jarigen dat tenminste vmbo gemengde leerweg of hoger heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>c16_havo</t>
-  </si>
-  <si>
-    <t>Volgt havo of hoger</t>
-  </si>
-  <si>
-    <t>het percentage 16-jarigen dat tenminste havo heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>c16_vwo</t>
-  </si>
-  <si>
-    <t>Volgt vwo</t>
-  </si>
-  <si>
-    <t>het percentage 16-jarigen dat vwo heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>c21_high_school_attained</t>
-  </si>
-  <si>
-    <t>21-jarige studenten</t>
-  </si>
-  <si>
-    <t>het percentage 21-jarigen dat een startkwalificatie heeft behaald (havo, vwo, of mbo niveau 2 of hoger).</t>
-  </si>
-  <si>
-    <t>c21_hbo_followed</t>
-  </si>
-  <si>
-    <t>het percentage 21-jarigen dat hbo en/of wo heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>C21_uni_followed</t>
-  </si>
-  <si>
-    <t>het percentage 21-jarigen dat wo heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>c30_hbo_attained</t>
-  </si>
-  <si>
-    <t>Diploma hbo of hoger</t>
-  </si>
-  <si>
-    <t>het percentage dertigers dat tenminste een hbo-diploma heeft behaald.</t>
-  </si>
-  <si>
-    <t>c30_wo_attained</t>
-  </si>
-  <si>
-    <t>Diploma universiteit</t>
-  </si>
-  <si>
-    <t>het percentage 21-jarigen dat tenminste een wo bachelordiploma heeft behaald.</t>
-  </si>
-  <si>
-    <t>c30_income</t>
-  </si>
-  <si>
-    <t>Persoonlijk inkomen</t>
-  </si>
-  <si>
-    <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
-  </si>
-  <si>
-    <t>c30_hourly_wage</t>
-  </si>
-  <si>
-    <t>Uurloon</t>
-  </si>
-  <si>
-    <t>het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017-2018 te delen door het aantal gewerkte basisuren.</t>
-  </si>
-  <si>
-    <t>c30_hrs_work_pw</t>
-  </si>
-  <si>
-    <t>Uren werk per week</t>
-  </si>
-  <si>
-    <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst, berekend door het aantal gewerkte basisuren in 2017 en 2018 te delen door 104.</t>
-  </si>
-  <si>
-    <t>c30_flex_contract</t>
-  </si>
-  <si>
-    <t>Flexibel arbeidscontract</t>
-  </si>
-  <si>
-    <t>het percentage dertigers in loondienst dat geen contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
-  </si>
-  <si>
-    <t>c30_employed</t>
-  </si>
-  <si>
-    <t>Werkend</t>
-  </si>
-  <si>
-    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
-  </si>
-  <si>
-    <t>c30_social_assistance</t>
-  </si>
-  <si>
-    <t>Bijstand</t>
-  </si>
-  <si>
-    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
-  </si>
-  <si>
-    <t>c30_disability</t>
-  </si>
-  <si>
-    <t>Uitkering arbeidsongeschiktheid/ziekte</t>
-  </si>
-  <si>
-    <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
-  </si>
-  <si>
-    <t>c30_debt</t>
-  </si>
-  <si>
-    <t>Schulden</t>
-  </si>
-  <si>
-    <t>het percentage dertigers met een negatief vermogen.</t>
-  </si>
-  <si>
-    <t>c11_living_space_pp</t>
-  </si>
-  <si>
-    <t>Woonoppervlak per lid van kinderen</t>
-  </si>
-  <si>
-    <t>het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8</t>
-  </si>
-  <si>
-    <t>c16_living_space_pp</t>
-  </si>
-  <si>
-    <t>Woonoppervlak per lid van tieners</t>
-  </si>
-  <si>
-    <t>het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
-  </si>
-  <si>
-    <t>c30_wealth</t>
-  </si>
-  <si>
-    <t>Vermogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertiger behoren in 2018. </t>
-  </si>
-  <si>
-    <t>c30_home_owner</t>
-  </si>
-  <si>
-    <t>Huiseigenaar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Het percentage dertigers met een koophuis in is eigenaar van een huis. </t>
-  </si>
-  <si>
-    <t>geografie</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Nederland</t>
-  </si>
-  <si>
-    <t>Metropool Amsterdam</t>
-  </si>
-  <si>
-    <t>Amsterdam</t>
-  </si>
-  <si>
-    <t>Gemeente</t>
-  </si>
-  <si>
-    <t>Almere</t>
-  </si>
-  <si>
-    <t>Amstelveen</t>
-  </si>
-  <si>
-    <t>Beverwijk</t>
-  </si>
-  <si>
-    <t>Gooise Meren</t>
-  </si>
-  <si>
-    <t>Haarlem</t>
-  </si>
-  <si>
-    <t>Haarlemmermeer</t>
-  </si>
-  <si>
-    <t>Lelystad</t>
-  </si>
-  <si>
-    <t>Purmerend</t>
-  </si>
-  <si>
-    <t>Velsen</t>
-  </si>
-  <si>
-    <t>Zaanstad</t>
-  </si>
-  <si>
-    <t>Edam-Volendam</t>
-  </si>
-  <si>
-    <t>Aalsmeer</t>
-  </si>
-  <si>
-    <t>Heemskerk</t>
-  </si>
-  <si>
-    <t>Hilversum</t>
-  </si>
-  <si>
-    <t>Huizen</t>
-  </si>
-  <si>
-    <t>Uithoorn</t>
-  </si>
-  <si>
-    <t>Bloemendaal</t>
-  </si>
-  <si>
-    <t>Heemstede</t>
-  </si>
-  <si>
-    <t>Wijdemeren</t>
-  </si>
-  <si>
-    <t>Wormerland</t>
-  </si>
-  <si>
-    <t>Diemen</t>
-  </si>
-  <si>
-    <t>Waterland</t>
-  </si>
-  <si>
-    <t>Weesp</t>
-  </si>
-  <si>
-    <t>Zuidoost</t>
-  </si>
-  <si>
-    <t>Stadsdeel</t>
-  </si>
-  <si>
-    <t>Noord</t>
-  </si>
-  <si>
-    <t>Oost</t>
-  </si>
-  <si>
-    <t>Nieuw-West</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-  <si>
-    <t>Centrum</t>
-  </si>
-  <si>
-    <t>Zuid</t>
-  </si>
-  <si>
-    <t>Gaasperdam, Driemond</t>
-  </si>
-  <si>
-    <t>Wijk</t>
-  </si>
-  <si>
-    <t>Noord-Oost</t>
-  </si>
-  <si>
-    <t>Bijlmer-Centrum, Amstel III</t>
-  </si>
-  <si>
-    <t>Indische Buurt, Oostelijk Havengebied</t>
-  </si>
-  <si>
-    <t>De Pijp, Rivierenbuurt</t>
-  </si>
-  <si>
-    <t>De Aker, Sloten, Nieuw-Sloten</t>
-  </si>
-  <si>
-    <t>Geuzenveld, Slotermeer, Sloterdijken</t>
-  </si>
-  <si>
-    <t>Osdorp</t>
-  </si>
-  <si>
-    <t>Bijlmer-Oost</t>
-  </si>
-  <si>
-    <t>Oud-Oost</t>
-  </si>
-  <si>
-    <t>Slotervaart</t>
-  </si>
-  <si>
-    <t>Noord-West</t>
-  </si>
-  <si>
-    <t>Bos en Lommer</t>
-  </si>
-  <si>
-    <t>IJburg, Zeeburgereiland</t>
-  </si>
-  <si>
-    <t>Oud West, De Baarsjes</t>
-  </si>
-  <si>
-    <t>Oud-Zuid</t>
-  </si>
-  <si>
-    <t>Oud-Noord</t>
-  </si>
-  <si>
-    <t>Westerpark</t>
-  </si>
-  <si>
-    <t>Centrum-Oost</t>
-  </si>
-  <si>
-    <t>Watergraafsmeer</t>
-  </si>
-  <si>
-    <t>Uitgeest</t>
-  </si>
-  <si>
-    <t>Zandvoort</t>
-  </si>
-  <si>
-    <t>Ouder-Amstel</t>
-  </si>
-  <si>
-    <t>Beemster</t>
-  </si>
-  <si>
-    <t>Landsmeer</t>
-  </si>
-  <si>
-    <t>Oostzaan</t>
-  </si>
-  <si>
-    <t>Blaricum</t>
-  </si>
-  <si>
-    <t>Laren</t>
-  </si>
-  <si>
-    <t>Centrum-West</t>
-  </si>
-  <si>
-    <t>Buitenveldert, Zuidas</t>
-  </si>
-  <si>
-    <t>Gezondheid en Welzijn</t>
-  </si>
-  <si>
-    <t>Onderwijs</t>
-  </si>
-  <si>
-    <t>Geld</t>
-  </si>
-  <si>
-    <t>Wonen</t>
-  </si>
-  <si>
-    <t>Startkwalificatie behaald</t>
-  </si>
-  <si>
-    <t>Volgend/gevolgd hbo of hoger</t>
-  </si>
-  <si>
-    <t>Volgend/gevolgd universiteit</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D204B-9EFA-3D41-9D75-AECB47552519}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1148,301 +1148,301 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1450,91 +1450,91 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>217</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -1545,7 +1545,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>11</v>
@@ -1568,7 +1568,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>14</v>
@@ -1585,25 +1585,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1614,7 +1614,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>17</v>
@@ -1632,508 +1632,508 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="G30" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="G32" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="G33" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="G35" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>132</v>
+        <v>212</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="G43" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>135</v>
+        <v>213</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2157,514 +2157,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ggtitle to fig and cleaned download data
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E0695B-9E88-A64D-A125-6C40EB4135E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE08EA7-F18F-5842-BBD9-6FD60EF09D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="219">
   <si>
     <t>analyse_outcome</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t xml:space="preserve">Het percentage dertigers met een koophuis. </t>
+  </si>
+  <si>
+    <t>het percentage  leerlingen in groep 8 met een leesvaardigheidscore van tenminste het streefniveau (2F) op de eindtoets.</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D204B-9EFA-3D41-9D75-AECB47552519}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1687,7 +1690,7 @@
         <v>204</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>63</v>
+        <v>218</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
change dashboard based on Bastian Feedback
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kco_dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE08EA7-F18F-5842-BBD9-6FD60EF09D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAEEE41-3CAC-CE42-83C1-AA904908409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
-    <sheet name="outcome" sheetId="3" r:id="rId1"/>
+    <sheet name="outcome" sheetId="4" r:id="rId1"/>
     <sheet name="area" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="220">
   <si>
     <t>analyse_outcome</t>
   </si>
@@ -94,12 +94,6 @@
     <t>c11_youth_health_costs</t>
   </si>
   <si>
-    <t>leerlingen van groep 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">700 duizend </t>
-  </si>
-  <si>
     <t>2003-2006</t>
   </si>
   <si>
@@ -115,9 +109,6 @@
     <t>c16_youth_health_costs</t>
   </si>
   <si>
-    <t>16-jarige scholieren</t>
-  </si>
-  <si>
     <t>1 miljoen</t>
   </si>
   <si>
@@ -151,18 +142,12 @@
     <t>c30_basic_mhc</t>
   </si>
   <si>
-    <t>Geestelijke gezondheidszorg (basis)</t>
-  </si>
-  <si>
     <t>het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (basis), vergoed vanuit de Zorgverzekeringswet.</t>
   </si>
   <si>
     <t>c30_specialist_mhc</t>
   </si>
   <si>
-    <t>Geestelijke gezondheidszorg (specialistisch)</t>
-  </si>
-  <si>
     <t>Het percentage van dertigers dat in 2018 gebruikt maakte van geestelijke gezondheidszorg (specialistisch), vergoed vanuit de Zorgverzekeringswet.</t>
   </si>
   <si>
@@ -310,9 +295,6 @@
     <t>c21_high_school_attained</t>
   </si>
   <si>
-    <t>21-jarige studenten</t>
-  </si>
-  <si>
     <t>het percentage 21-jarigen dat een startkwalificatie heeft behaald (havo, vwo, of mbo niveau 2 of hoger).</t>
   </si>
   <si>
@@ -646,9 +628,6 @@
     <t>Buitenveldert, Zuidas</t>
   </si>
   <si>
-    <t>Gezondheid en Welzijn</t>
-  </si>
-  <si>
     <t>Onderwijs</t>
   </si>
   <si>
@@ -661,12 +640,6 @@
     <t>Startkwalificatie behaald</t>
   </si>
   <si>
-    <t>Volgend/gevolgd hbo of hoger</t>
-  </si>
-  <si>
-    <t>Volgend/gevolgd universiteit</t>
-  </si>
-  <si>
     <t>Woonoppervlak per lid van kinderen</t>
   </si>
   <si>
@@ -692,6 +665,36 @@
   </si>
   <si>
     <t>het percentage  leerlingen in groep 8 met een leesvaardigheidscore van tenminste het streefniveau (2F) op de eindtoets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710 duizend </t>
+  </si>
+  <si>
+    <t>Gebruikt geestelijke gezondheidszorg (specialistisch)</t>
+  </si>
+  <si>
+    <t>Gebruikt geestelijke gezondheidszorg (basis)</t>
+  </si>
+  <si>
+    <t>leerlingen groep 8</t>
+  </si>
+  <si>
+    <t>21-jarigen</t>
+  </si>
+  <si>
+    <t>16-jarigen</t>
+  </si>
+  <si>
+    <t>968 duizend</t>
+  </si>
+  <si>
+    <t>Gezondheid en welzijn</t>
+  </si>
+  <si>
+    <t>Volgend/ gevolgd hbo of hoger</t>
+  </si>
+  <si>
+    <t>Volgend/ gevolgd universiteit</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +761,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -774,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -793,6 +802,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,19 +1124,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D204B-9EFA-3D41-9D75-AECB47552519}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A5AA57-5D7B-1344-9D5A-874482A966DC}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -1126,7 +1144,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1149,53 +1167,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>198</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
@@ -1203,378 +1221,378 @@
         <v>103</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="C18" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="B19" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="E19" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C20" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>8</v>
@@ -1586,557 +1604,557 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="13" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>97</v>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>34</v>
+        <v>213</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>27</v>
+        <v>210</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>100</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="G37" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="C38" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>28</v>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2160,514 +2178,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change outcome names to values and labels
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAEEE41-3CAC-CE42-83C1-AA904908409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9705F95D-9B29-1B49-8B8D-5DA568A98690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="-35840" yWindow="-2800" windowWidth="34500" windowHeight="18820" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="216">
   <si>
     <t>analyse_outcome</t>
   </si>
@@ -640,24 +640,6 @@
     <t>Startkwalificatie behaald</t>
   </si>
   <si>
-    <t>Woonoppervlak per lid van kinderen</t>
-  </si>
-  <si>
-    <t>Woonoppervlak per lid van tieners</t>
-  </si>
-  <si>
-    <t>Jeugd zorgkosten van kinderen</t>
-  </si>
-  <si>
-    <t>Jeugd zorgkosten van tieners</t>
-  </si>
-  <si>
-    <t>Jeugdbescherming van kinderen</t>
-  </si>
-  <si>
-    <t>Jeugdbescherming van tieners</t>
-  </si>
-  <si>
     <t>het percentage 21-jarigen dat tenminste een wo bachelorsdiploma heeft behaald.</t>
   </si>
   <si>
@@ -695,6 +677,12 @@
   </si>
   <si>
     <t>Volgend/ gevolgd universiteit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeugdbescherming </t>
+  </si>
+  <si>
+    <t>Woonoppervlak per lid huishouden</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1116,10 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -1144,7 +1132,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>96</v>
       </c>
@@ -1190,7 +1178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>108</v>
       </c>
@@ -1213,7 +1201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
@@ -1236,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>105</v>
       </c>
@@ -1259,7 +1247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>99</v>
       </c>
@@ -1282,7 +1270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>114</v>
       </c>
@@ -1305,7 +1293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -1328,7 +1316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>124</v>
       </c>
@@ -1351,7 +1339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>117</v>
       </c>
@@ -1374,7 +1362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1382,7 +1370,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>33</v>
@@ -1397,7 +1385,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1405,7 +1393,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>40</v>
@@ -1420,15 +1408,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>217</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>37</v>
@@ -1443,15 +1431,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>35</v>
@@ -1466,7 +1454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1474,7 +1462,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>43</v>
@@ -1489,44 +1477,44 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>203</v>
+        <v>30</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>204</v>
+        <v>30</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>24</v>
@@ -1535,44 +1523,44 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>24</v>
@@ -1581,7 +1569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1589,7 +1577,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>11</v>
@@ -1604,7 +1592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1612,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>14</v>
@@ -1627,7 +1615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1623,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>17</v>
@@ -1651,7 +1639,7 @@
       </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>44</v>
       </c>
@@ -1665,16 +1653,16 @@
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>47</v>
       </c>
@@ -1688,16 +1676,16 @@
         <v>49</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>50</v>
       </c>
@@ -1711,16 +1699,16 @@
         <v>52</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>53</v>
       </c>
@@ -1734,16 +1722,16 @@
         <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>56</v>
       </c>
@@ -1754,19 +1742,19 @@
         <v>197</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>59</v>
       </c>
@@ -1780,16 +1768,16 @@
         <v>58</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>61</v>
       </c>
@@ -1803,16 +1791,16 @@
         <v>63</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>64</v>
       </c>
@@ -1826,16 +1814,16 @@
         <v>66</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>67</v>
       </c>
@@ -1849,16 +1837,16 @@
         <v>69</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>70</v>
       </c>
@@ -1872,16 +1860,16 @@
         <v>72</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>73</v>
       </c>
@@ -1895,16 +1883,16 @@
         <v>75</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>76</v>
       </c>
@@ -1918,7 +1906,7 @@
         <v>78</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>24</v>
@@ -1927,7 +1915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>79</v>
       </c>
@@ -1941,7 +1929,7 @@
         <v>81</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>24</v>
@@ -1950,7 +1938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>82</v>
       </c>
@@ -1964,7 +1952,7 @@
         <v>84</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>24</v>
@@ -1973,7 +1961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>85</v>
       </c>
@@ -1987,21 +1975,21 @@
         <v>86</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>197</v>
@@ -2010,21 +1998,21 @@
         <v>88</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>89</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>197</v>
@@ -2033,16 +2021,16 @@
         <v>90</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
@@ -2065,7 +2053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>94</v>
       </c>
@@ -2076,7 +2064,7 @@
         <v>197</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>31</v>
@@ -2088,7 +2076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>127</v>
       </c>
@@ -2099,7 +2087,7 @@
         <v>199</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>31</v>
@@ -2111,12 +2099,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>120</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>199</v>
@@ -2125,21 +2113,21 @@
         <v>121</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>122</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>199</v>
@@ -2148,7 +2136,7 @@
         <v>123</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
fix few typos in outcome names
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9705F95D-9B29-1B49-8B8D-5DA568A98690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497A811C-9012-EF4D-B72E-CDF2FE5CFEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35840" yWindow="-2800" windowWidth="34500" windowHeight="18820" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -304,9 +304,6 @@
     <t>het percentage 21-jarigen dat hbo en/of wo heeft gevolgd.</t>
   </si>
   <si>
-    <t>C21_uni_followed</t>
-  </si>
-  <si>
     <t>het percentage 21-jarigen dat wo heeft gevolgd.</t>
   </si>
   <si>
@@ -683,6 +680,9 @@
   </si>
   <si>
     <t>Woonoppervlak per lid huishouden</t>
+  </si>
+  <si>
+    <t>c21_uni_followed</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A5AA57-5D7B-1344-9D5A-874482A966DC}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1157,16 +1157,16 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>31</v>
@@ -1180,16 +1180,16 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>31</v>
@@ -1203,16 +1203,16 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>31</v>
@@ -1226,16 +1226,16 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>31</v>
@@ -1249,16 +1249,16 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>31</v>
@@ -1272,16 +1272,16 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>31</v>
@@ -1295,16 +1295,16 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>31</v>
@@ -1318,16 +1318,16 @@
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="C9" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>125</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>126</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>31</v>
@@ -1341,16 +1341,16 @@
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>31</v>
@@ -1370,7 +1370,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>33</v>
@@ -1393,7 +1393,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>40</v>
@@ -1413,10 +1413,10 @@
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>37</v>
@@ -1436,10 +1436,10 @@
         <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>35</v>
@@ -1462,7 +1462,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>43</v>
@@ -1485,16 +1485,16 @@
         <v>30</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>19</v>
@@ -1508,13 +1508,13 @@
         <v>30</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>24</v>
@@ -1528,19 +1528,19 @@
         <v>21</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>19</v>
@@ -1551,16 +1551,16 @@
         <v>27</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>24</v>
@@ -1577,7 +1577,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>11</v>
@@ -1600,7 +1600,7 @@
         <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>14</v>
@@ -1623,7 +1623,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>17</v>
@@ -1647,16 +1647,16 @@
         <v>45</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>19</v>
@@ -1670,16 +1670,16 @@
         <v>48</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>19</v>
@@ -1693,16 +1693,16 @@
         <v>51</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>19</v>
@@ -1716,16 +1716,16 @@
         <v>54</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>19</v>
@@ -1739,16 +1739,16 @@
         <v>57</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>19</v>
@@ -1762,16 +1762,16 @@
         <v>60</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>19</v>
@@ -1785,16 +1785,16 @@
         <v>62</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>19</v>
@@ -1808,16 +1808,16 @@
         <v>65</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>19</v>
@@ -1831,16 +1831,16 @@
         <v>68</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>19</v>
@@ -1854,16 +1854,16 @@
         <v>71</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>19</v>
@@ -1877,16 +1877,16 @@
         <v>74</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>19</v>
@@ -1900,13 +1900,13 @@
         <v>77</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>24</v>
@@ -1923,13 +1923,13 @@
         <v>80</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>24</v>
@@ -1946,13 +1946,13 @@
         <v>83</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>24</v>
@@ -1966,19 +1966,19 @@
         <v>85</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>86</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>25</v>
@@ -1989,19 +1989,19 @@
         <v>87</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>88</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>25</v>
@@ -2009,22 +2009,22 @@
     </row>
     <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="E39" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>25</v>
@@ -2032,16 +2032,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>31</v>
@@ -2055,16 +2055,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="C41" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>31</v>
@@ -2078,16 +2078,16 @@
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="C42" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>31</v>
@@ -2101,22 +2101,22 @@
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>121</v>
-      </c>
       <c r="E43" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>19</v>
@@ -2124,19 +2124,19 @@
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="D44" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>123</v>
-      </c>
       <c r="E44" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F44" s="14" t="s">
         <v>24</v>
@@ -2166,514 +2166,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change order of outcome dropdown menu
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0422DFB6-120E-404B-A797-DE9E4D5436A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FB5C5B-1A0C-A840-B6AB-9423620419D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
-    <sheet name="outcome" sheetId="4" r:id="rId1"/>
+    <sheet name="outcome" sheetId="5" r:id="rId1"/>
     <sheet name="area" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -664,12 +664,6 @@
     <t>Gezondheid en welzijn</t>
   </si>
   <si>
-    <t>Volgend/ gevolgd hbo of hoger</t>
-  </si>
-  <si>
-    <t>Volgend/ gevolgd universiteit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jeugdbescherming </t>
   </si>
   <si>
@@ -695,6 +689,12 @@
   </si>
   <si>
     <t>het gemiddelde totale schulden van huishouden waartoe dertigers behoren in 2018.</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd hbo of hoger</t>
+  </si>
+  <si>
+    <t>Volgend/gevolgd universiteit</t>
   </si>
 </sst>
 </file>
@@ -751,7 +751,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,12 +761,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -801,19 +795,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1127,30 +1112,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A5AA57-5D7B-1344-9D5A-874482A966DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5108B3D-FFAF-614D-935E-1C1C3F2BF8F8}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="164" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="21.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="115.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="112.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1173,270 +1156,275 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>215</v>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>97</v>
+        <v>208</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>195</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>209</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>24</v>
+        <v>204</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>100</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>24</v>
+        <v>204</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="F9" s="12" t="s">
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
+      <c r="E11" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>38</v>
@@ -1453,554 +1441,564 @@
       <c r="F12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>202</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>208</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>214</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>35</v>
+        <v>194</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>24</v>
+        <v>204</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>214</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
+        <v>194</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>24</v>
+        <v>204</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="12" t="s">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G17" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>214</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>9</v>
+        <v>204</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
+        <v>214</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>9</v>
+        <v>204</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>194</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="12" t="s">
         <v>201</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>194</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="12" t="s">
         <v>201</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
+        <v>76</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>194</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>201</v>
+        <v>78</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>214</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>201</v>
+        <v>81</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>56</v>
+        <v>214</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>201</v>
+        <v>84</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>58</v>
+      <c r="E28" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>201</v>
+        <v>205</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>201</v>
+        <v>205</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>64</v>
+        <v>211</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>201</v>
+        <v>205</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>207</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>67</v>
+        <v>214</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>70</v>
+        <v>214</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>194</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>72</v>
+        <v>198</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>201</v>
+        <v>31</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>75</v>
+        <v>210</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="12" t="s">
         <v>201</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -2009,24 +2007,24 @@
     </row>
     <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>78</v>
+        <v>215</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H34" s="2" t="s">
@@ -2035,24 +2033,24 @@
     </row>
     <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G35" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H35" s="2" t="s">
@@ -2060,25 +2058,25 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>82</v>
+      <c r="A36" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G36" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -2086,129 +2084,129 @@
       </c>
     </row>
     <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="H37" s="12" t="s">
+      <c r="A37" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="H38" s="12" t="s">
+    <row r="38" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B39" s="11" t="s">
+      <c r="A39" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E39" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>194</v>
+        <v>99</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="16" t="s">
+      <c r="G40" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>194</v>
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>198</v>
+        <v>115</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G41" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H41" s="2" t="s">
@@ -2216,80 +2214,80 @@
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="F42" s="12" t="s">
+      <c r="F43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="17" t="s">
+      <c r="G43" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H42" s="12" t="s">
+      <c r="H43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="12" t="s">
+    <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G44" s="17" t="s">
+      <c r="F44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H44" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add dynamic text in wat zie ik? for opleiding ouders
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF1CA84-6396-9A42-9AF4-E2E58BB3616E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C82871A-7644-FD4E-BF8B-C8E283DA15A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -463,9 +463,6 @@
     <t>Onderwijs</t>
   </si>
   <si>
-    <t>Geld</t>
-  </si>
-  <si>
     <t>Wonen</t>
   </si>
   <si>
@@ -478,9 +475,6 @@
     <t>Gebruikt geestelijke gezondheidszorg (basis)</t>
   </si>
   <si>
-    <t>leerlingen groep 8</t>
-  </si>
-  <si>
     <t>21-jarigen</t>
   </si>
   <si>
@@ -1777,6 +1771,12 @@
       </rPr>
       <t>waartoe dertigers behoren in 2018.</t>
     </r>
+  </si>
+  <si>
+    <t>Werk en inkomen</t>
+  </si>
+  <si>
+    <t>leerlingen in groep 8</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2225,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -2261,10 +2261,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
@@ -2279,7 +2279,7 @@
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -2288,10 +2288,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>8</v>
@@ -2306,7 +2306,7 @@
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -2315,10 +2315,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
@@ -2341,16 +2341,16 @@
         <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>16</v>
@@ -2358,25 +2358,25 @@
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>16</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -2394,13 +2394,13 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>19</v>
@@ -2411,22 +2411,22 @@
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>19</v>
@@ -2438,19 +2438,19 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>24</v>
@@ -2464,19 +2464,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>24</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
@@ -2499,10 +2499,10 @@
         <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>24</v>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>28</v>
@@ -2525,10 +2525,10 @@
         <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>24</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>22</v>
@@ -2551,10 +2551,10 @@
         <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>24</v>
@@ -2569,25 +2569,25 @@
     </row>
     <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>16</v>
@@ -2596,25 +2596,25 @@
     </row>
     <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>16</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>34</v>
@@ -2635,13 +2635,13 @@
         <v>141</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>16</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>36</v>
@@ -2662,13 +2662,13 @@
         <v>141</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>16</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
@@ -2689,13 +2689,13 @@
         <v>141</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>16</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>40</v>
@@ -2716,13 +2716,13 @@
         <v>141</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>16</v>
@@ -2731,25 +2731,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>16</v>
@@ -2757,25 +2757,25 @@
     </row>
     <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>16</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>44</v>
@@ -2796,13 +2796,13 @@
         <v>141</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>16</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>46</v>
@@ -2822,13 +2822,13 @@
         <v>141</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>16</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>48</v>
@@ -2849,13 +2849,13 @@
         <v>141</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>16</v>
@@ -2863,22 +2863,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>19</v>
@@ -2889,22 +2889,22 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>19</v>
@@ -2915,22 +2915,22 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>19</v>
@@ -2941,25 +2941,25 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>20</v>
@@ -2967,25 +2967,25 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>20</v>
@@ -2993,25 +2993,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>20</v>
@@ -3019,19 +3019,19 @@
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>24</v>
@@ -3046,19 +3046,19 @@
     </row>
     <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>24</v>
@@ -3073,25 +3073,25 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>16</v>
@@ -3099,22 +3099,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>19</v>
@@ -3125,19 +3125,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>24</v>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>57</v>
@@ -3160,10 +3160,10 @@
         <v>58</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>24</v>
@@ -3177,19 +3177,19 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>24</v>
@@ -3203,19 +3203,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>24</v>
@@ -3229,19 +3229,19 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>211</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>24</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>59</v>
@@ -3264,10 +3264,10 @@
         <v>60</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>24</v>
@@ -3281,19 +3281,19 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>24</v>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>63</v>
@@ -3316,10 +3316,10 @@
         <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>24</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>70</v>
@@ -3342,10 +3342,10 @@
         <v>71</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>24</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>66</v>
@@ -3368,10 +3368,10 @@
         <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
add whitespace in outcome explanation c21_hbo_followed
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C82871A-7644-FD4E-BF8B-C8E283DA15A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DFA4D-795D-8746-A478-BC359FD019AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -1235,6 +1235,54 @@
     <t xml:space="preserve">Hbo of hoger </t>
   </si>
   <si>
+    <t xml:space="preserve">Universiteit </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">het percentage 21-jarigen dat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">een universitaire opleiding </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>heeft gevolgd.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Diploma hbo of hoger </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1253,17 +1301,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het percentage 21-jarigen dat een hbo- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>of</t>
+      <t xml:space="preserve"> het percentage dertigers dat  een hbo- of universitair diploma heeft behaald.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Diploma universiteit </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">het percentage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dertigers</t>
     </r>
     <r>
       <rPr>
@@ -1283,30 +1356,95 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>universitaire opleiding</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> heeft gevolgd.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Universiteit </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+      <t>dat een</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> universitair diploma heeft behaald.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Eigen woning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">et percentage dertigers met een koophuis. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">is </t>
     </r>
@@ -1316,33 +1454,128 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">het percentage 21-jarigen dat </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">een universitaire opleiding </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>heeft gevolgd.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Diploma hbo of hoger </t>
+      </rPr>
+      <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
+    </r>
+  </si>
+  <si>
+    <t>Werkt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gewerkte uren per week (werkenden)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst in 2017 en 2018.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c30_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>permanent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_contract</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arbeidscontract</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers in loondienst dat een contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1363,11 +1596,33 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het percentage dertigers dat  een hbo- of universitair diploma heeft behaald.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Diploma universiteit </t>
+      <t xml:space="preserve"> het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017-2018 te delen door het aantal gewerkte basisuren.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1388,47 +1643,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">het percentage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dertigers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dat een</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> universitair diploma heeft behaald.</t>
+      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
     </r>
   </si>
   <si>
@@ -1450,305 +1687,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
-    </r>
-  </si>
-  <si>
-    <t>Eigen woning</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">et percentage dertigers met een koophuis. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
-    </r>
-  </si>
-  <si>
-    <t>Werkt</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
-    </r>
-  </si>
-  <si>
-    <t>Gewerkte uren per week (werkenden)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst in 2017 en 2018.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c30_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>permanent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_contract</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arbeidscontract</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers in loondienst dat een contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017-2018 te delen door het aantal gewerkte basisuren.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> het gemiddelde </t>
     </r>
     <r>
@@ -1777,6 +1715,9 @@
   </si>
   <si>
     <t>leerlingen in groep 8</t>
+  </si>
+  <si>
+    <t>is het percentage 21-jarigen dat een hbo- of universitaire opleiding heeft gevolgd.</t>
   </si>
 </sst>
 </file>
@@ -2207,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="128.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2347,7 +2288,7 @@
         <v>161</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>143</v>
@@ -2373,7 +2314,7 @@
         <v>160</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>143</v>
@@ -2584,7 +2525,7 @@
         <v>170</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>143</v>
@@ -2611,7 +2552,7 @@
         <v>172</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>143</v>
@@ -2638,7 +2579,7 @@
         <v>173</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>143</v>
@@ -2665,7 +2606,7 @@
         <v>174</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>143</v>
@@ -2692,7 +2633,7 @@
         <v>175</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>143</v>
@@ -2719,7 +2660,7 @@
         <v>176</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>143</v>
@@ -2746,7 +2687,7 @@
         <v>178</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>143</v>
@@ -2772,7 +2713,7 @@
         <v>180</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>143</v>
@@ -2799,7 +2740,7 @@
         <v>181</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>143</v>
@@ -2825,7 +2766,7 @@
         <v>182</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>143</v>
@@ -2852,7 +2793,7 @@
         <v>183</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>143</v>
@@ -2979,7 +2920,7 @@
         <v>141</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>146</v>
@@ -2999,13 +2940,13 @@
         <v>152</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>146</v>
@@ -3025,13 +2966,13 @@
         <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>24</v>
@@ -3052,13 +2993,13 @@
         <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>24</v>
@@ -3085,10 +3026,10 @@
         <v>142</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>143</v>
@@ -3111,7 +3052,7 @@
         <v>142</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>147</v>
@@ -3131,13 +3072,13 @@
         <v>72</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>142</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>24</v>
@@ -3160,10 +3101,10 @@
         <v>58</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>24</v>
@@ -3183,13 +3124,13 @@
         <v>62</v>
       </c>
       <c r="C37" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>24</v>
@@ -3209,13 +3150,13 @@
         <v>61</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>24</v>
@@ -3232,16 +3173,16 @@
         <v>155</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>24</v>
@@ -3264,10 +3205,10 @@
         <v>60</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>24</v>
@@ -3287,13 +3228,13 @@
         <v>65</v>
       </c>
       <c r="C41" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>213</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>214</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>24</v>
@@ -3316,10 +3257,10 @@
         <v>64</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>24</v>
@@ -3342,10 +3283,10 @@
         <v>71</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>24</v>
@@ -3368,10 +3309,10 @@
         <v>67</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
change new doc werkwijze
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DFA4D-795D-8746-A478-BC359FD019AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A98E9-365F-E549-AB97-FFDB1E22628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
+    <workbookView xWindow="-33300" yWindow="-280" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
   <sheets>
     <sheet name="outcome" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="210">
   <si>
     <t>analyse_outcome</t>
   </si>
@@ -49,12 +49,6 @@
     <t>population</t>
   </si>
   <si>
-    <t>sample_size</t>
-  </si>
-  <si>
-    <t>birth_year</t>
-  </si>
-  <si>
     <t>c00_sga</t>
   </si>
   <si>
@@ -64,12 +58,6 @@
     <t>pasgeborenen</t>
   </si>
   <si>
-    <t>1,4 miljoen</t>
-  </si>
-  <si>
-    <t>2008-2016</t>
-  </si>
-  <si>
     <t>c00_preterm_birth</t>
   </si>
   <si>
@@ -85,21 +73,12 @@
     <t>c11_youth_health_costs</t>
   </si>
   <si>
-    <t>2003-2006</t>
-  </si>
-  <si>
     <t>c11_youth_protection</t>
   </si>
   <si>
     <t>c16_youth_health_costs</t>
   </si>
   <si>
-    <t>1 miljoen</t>
-  </si>
-  <si>
-    <t>1998-2002</t>
-  </si>
-  <si>
     <t>c16_youth_protection</t>
   </si>
   <si>
@@ -112,9 +91,6 @@
     <t>dertigers</t>
   </si>
   <si>
-    <t>1982-1987</t>
-  </si>
-  <si>
     <t>c30_basic_mhc</t>
   </si>
   <si>
@@ -466,9 +442,6 @@
     <t>Wonen</t>
   </si>
   <si>
-    <t xml:space="preserve">710 duizend </t>
-  </si>
-  <si>
     <t>Gebruikt geestelijke gezondheidszorg (specialistisch)</t>
   </si>
   <si>
@@ -481,9 +454,6 @@
     <t>16-jarigen</t>
   </si>
   <si>
-    <t>968 duizend</t>
-  </si>
-  <si>
     <t>Gezondheid en welzijn</t>
   </si>
   <si>
@@ -1578,6 +1548,9 @@
     </r>
   </si>
   <si>
+    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1596,11 +1569,52 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017-2018 te delen door het aantal gewerkte basisuren.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
+      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
+    </r>
   </si>
   <si>
     <r>
@@ -1621,72 +1635,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> het gemiddelde </t>
     </r>
     <r>
@@ -1718,13 +1666,16 @@
   </si>
   <si>
     <t>is het percentage 21-jarigen dat een hbo- of universitaire opleiding heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>is het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017 en 2018 te delen door het aantal gewerkte basisuren.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1769,12 +1720,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1813,7 +1758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1823,12 +1768,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2146,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="128.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2160,13 +2104,11 @@
     <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="127.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2175,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -2183,1145 +2125,881 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="F13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="D36" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="D40" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="D42" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="C44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3345,514 +3023,514 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dot in description in outcome table
</commit_message>
<xml_diff>
--- a/data/outcome_table.xlsx
+++ b/data/outcome_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenlam20/GitHub/kenniscentrumongelijkheid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A98E9-365F-E549-AB97-FFDB1E22628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1C84D6-7D4C-0948-9734-B22B0EE1FAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33300" yWindow="-280" windowWidth="28800" windowHeight="17500" xr2:uid="{F41B97FE-F77A-4840-B0FB-A5C2C3F09623}"/>
   </bookViews>
@@ -1358,8 +1358,175 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8</t>
-    </r>
+      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Eigen woning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">et percentage dertigers met een koophuis. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
+    </r>
+  </si>
+  <si>
+    <t>Werkt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
+    </r>
+  </si>
+  <si>
+    <t>Gewerkte uren per week (werkenden)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst in 2017 en 2018.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c30_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>permanent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_contract</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> arbeidscontract</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers in loondienst dat een contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
   </si>
   <si>
     <r>
@@ -1380,41 +1547,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van 16-jarigen.</t>
-    </r>
-  </si>
-  <si>
-    <t>Eigen woning</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>h</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">et percentage dertigers met een koophuis. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">is </t>
     </r>
@@ -1424,12 +1567,10 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t>het gemiddelde bruto persoonlijk jaarinkomen in 2017 en 2018 (prijspeil van 2018). </t>
-    </r>
-  </si>
-  <si>
-    <t>Werkt</t>
+        <scheme val="minor"/>
+      </rPr>
+      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1450,105 +1591,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit werk ontving.</t>
-    </r>
-  </si>
-  <si>
-    <t>Gewerkte uren per week (werkenden)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het gemiddelde aantal gewerkte uren per week van dertigers in loondienst in 2017 en 2018.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>c30_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>permanent</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_contract</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> arbeidscontract</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers in loondienst dat een contract voor onbepaalde tijd had in de langstlopende baan in 2017 en 2018.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ziekte- of arbeidsongeschiktheidsuitkering</t>
+      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
+    </r>
   </si>
   <si>
     <r>
@@ -1569,52 +1613,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het percentage dertigers dat in december 2018 het meeste inkomen uit een ziekte- of arbeidsongeschiktheidsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>het percentage dertigers dat in december 2018 het meeste inkomen uit een bijstandsuitkering ontving.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">het totale vermogen van het huishouden waartoe dertigers behoren in 2018. </t>
-    </r>
+      <t xml:space="preserve"> het gemiddelde </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">van de totale schulden van het huishouden </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>waartoe dertigers behoren in 2018.</t>
+    </r>
+  </si>
+  <si>
+    <t>Werk en inkomen</t>
+  </si>
+  <si>
+    <t>leerlingen in groep 8</t>
+  </si>
+  <si>
+    <t>is het percentage 21-jarigen dat een hbo- of universitaire opleiding heeft gevolgd.</t>
+  </si>
+  <si>
+    <t>is het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017 en 2018 te delen door het aantal gewerkte basisuren.</t>
   </si>
   <si>
     <r>
@@ -1635,40 +1667,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> het gemiddelde </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">van de totale schulden van het huishouden </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>waartoe dertigers behoren in 2018.</t>
-    </r>
-  </si>
-  <si>
-    <t>Werk en inkomen</t>
-  </si>
-  <si>
-    <t>leerlingen in groep 8</t>
-  </si>
-  <si>
-    <t>is het percentage 21-jarigen dat een hbo- of universitaire opleiding heeft gevolgd.</t>
-  </si>
-  <si>
-    <t>is het gemiddelde uurloon (prijspeil van 2018) van dertigers in loondienst, berekend door het basisloon over 2017 en 2018 te delen door het aantal gewerkte basisuren.</t>
+      <t xml:space="preserve"> het gemiddelde woonoppervlak per lid van het huishouden van leerlingen in groep 8.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2092,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F4A81B-7759-BE45-BE6A-975E9F190FD6}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="128.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2206,7 +2206,7 @@
         <v>151</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2226,7 +2226,7 @@
         <v>150</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G6"/>
     </row>
@@ -2389,7 +2389,7 @@
         <v>160</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G14"/>
     </row>
@@ -2410,7 +2410,7 @@
         <v>162</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G15"/>
     </row>
@@ -2431,7 +2431,7 @@
         <v>163</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G16"/>
     </row>
@@ -2452,7 +2452,7 @@
         <v>164</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G17"/>
     </row>
@@ -2473,7 +2473,7 @@
         <v>165</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G18"/>
     </row>
@@ -2494,7 +2494,7 @@
         <v>166</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G19"/>
     </row>
@@ -2515,7 +2515,7 @@
         <v>168</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2535,7 +2535,7 @@
         <v>170</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G21"/>
     </row>
@@ -2556,7 +2556,7 @@
         <v>171</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
         <v>172</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G23"/>
     </row>
@@ -2597,7 +2597,7 @@
         <v>173</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -2694,7 +2694,7 @@
         <v>133</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>137</v>
@@ -2776,10 +2776,10 @@
         <v>134</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2796,7 +2796,7 @@
         <v>134</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>138</v>
@@ -2810,13 +2810,13 @@
         <v>64</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>134</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>17</v>
@@ -2833,10 +2833,10 @@
         <v>50</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
@@ -2850,13 +2850,13 @@
         <v>54</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>195</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>17</v>
@@ -2870,13 +2870,13 @@
         <v>53</v>
       </c>
       <c r="C38" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>17</v>
@@ -2887,16 +2887,16 @@
         <v>145</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>17</v>
@@ -2913,10 +2913,10 @@
         <v>52</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>17</v>
@@ -2930,13 +2930,13 @@
         <v>57</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>17</v>
@@ -2953,10 +2953,10 @@
         <v>56</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>17</v>
@@ -2973,10 +2973,10 @@
         <v>63</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>17</v>
@@ -2993,10 +2993,10 @@
         <v>59</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>17</v>

</xml_diff>